<commit_message>
updated user story file.
</commit_message>
<xml_diff>
--- a/BankAPP-Employee User stories.xlsx
+++ b/BankAPP-Employee User stories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>SI</t>
   </si>
@@ -81,13 +81,19 @@
     <t>AS A Requester I WANT TO Know is rquest is placed or not SO THAT I or My Team can use to perform the duty.</t>
   </si>
   <si>
-    <t>AS A Requester I WANT TO check my account statement SO THAT I or My Team can use to perform the duty.</t>
-  </si>
-  <si>
     <t>AS A Requester I WANT TO Able to sned the feedback on the Item which was Issued SO THAT I or My Team can use to perform the duty.</t>
   </si>
   <si>
     <t>AS A Requester I WANT TO Change in my Address details SO THAT I can reach the product where it is required.</t>
+  </si>
+  <si>
+    <t>Epic</t>
+  </si>
+  <si>
+    <t>AS A Requester I WANT TO Track my item SO THAT i can easily Know when i get my item.</t>
+  </si>
+  <si>
+    <t>AS A Requester I WANT TO Able to modify my item list SO THAT i can do my work.</t>
   </si>
 </sst>
 </file>
@@ -419,199 +425,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="129.28515625" customWidth="1"/>
+    <col min="3" max="4" width="129.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="11.25" customHeight="1">
+    <row r="2" spans="1:3" ht="11.25" customHeight="1">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>22</v>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>